<commit_message>
Basic Transformation - Trying to combine data by using UNION ALL
</commit_message>
<xml_diff>
--- a/BasicTransformations/X Factor contestants.xlsx
+++ b/BasicTransformations/X Factor contestants.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Males" sheetId="2" r:id="rId2"/>
+    <sheet name="Females" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
   <si>
     <t xml:space="preserve">Series </t>
   </si>
@@ -411,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,4 +599,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4">
+        <v>38234</v>
+      </c>
+      <c r="D2" s="4">
+        <v>38332</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>38584</v>
+      </c>
+      <c r="D3" s="4">
+        <v>38703</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>39312</v>
+      </c>
+      <c r="D4" s="4">
+        <v>39431</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>40047</v>
+      </c>
+      <c r="D5" s="4">
+        <v>40160</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>40411</v>
+      </c>
+      <c r="D6" s="4">
+        <v>40524</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4">
+        <v>41139</v>
+      </c>
+      <c r="D7" s="4">
+        <v>41252</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4">
+        <v>38948</v>
+      </c>
+      <c r="D2" s="4">
+        <v>39067</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>39676</v>
+      </c>
+      <c r="D3" s="4">
+        <v>39795</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4">
+        <v>40775</v>
+      </c>
+      <c r="D4" s="4">
+        <v>40888</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>